<commit_message>
Adding ancient points to BOXPLOT-TRANSPORT
</commit_message>
<xml_diff>
--- a/Code/STATISTICS-AUTHOR.xlsx
+++ b/Code/STATISTICS-AUTHOR.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jocelynreahl/Documents/BergmannLab_2018-2020/Reahl_2020/Code/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535DB0F6-0316-F74A-9CEF-C5A3F793AB54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="440" windowWidth="14000" windowHeight="14180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -82,8 +76,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,7 +102,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -131,27 +125,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -160,14 +140,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -214,7 +186,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -246,27 +218,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -298,24 +252,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -491,16 +427,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -525,9 +459,8 @@
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -541,22 +474,22 @@
         <v>16</v>
       </c>
       <c r="E2">
-        <v>-2.0555124362421591</v>
+        <v>-2.055512436242159</v>
       </c>
       <c r="F2">
-        <v>6.8913663845058204E-2</v>
+        <v>0.0689136638450582</v>
       </c>
       <c r="G2">
         <v>1.554964003448891</v>
       </c>
       <c r="H2">
-        <v>-3.2128437814160771</v>
+        <v>-3.212843781416077</v>
       </c>
       <c r="I2">
-        <v>3.3673558541667772</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+        <v>3.367355854166777</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -573,19 +506,19 @@
         <v>-2.211360198655218</v>
       </c>
       <c r="F3">
-        <v>-2.0034243150019999</v>
+        <v>-2.003424315002</v>
       </c>
       <c r="G3">
-        <v>-1.8300564172848679</v>
+        <v>-1.830056417284868</v>
       </c>
       <c r="H3">
-        <v>-2.6188833714232218</v>
+        <v>-2.618883371423222</v>
       </c>
       <c r="I3">
-        <v>-1.4951284445754149</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+        <v>-1.495128444575415</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -602,19 +535,19 @@
         <v>-2.681103601788219</v>
       </c>
       <c r="F4">
-        <v>-0.78499135634333472</v>
+        <v>-0.7849913563433347</v>
       </c>
       <c r="G4">
-        <v>-0.25232125322382709</v>
+        <v>-0.2523212532238271</v>
       </c>
       <c r="H4">
-        <v>-3.1073990254294812</v>
+        <v>-3.107399025429481</v>
       </c>
       <c r="I4">
         <v>1.782707105295364</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -628,22 +561,22 @@
         <v>16</v>
       </c>
       <c r="E5">
-        <v>0.38530872082552498</v>
+        <v>0.385308720825525</v>
       </c>
       <c r="F5">
-        <v>1.1561708502841479</v>
+        <v>1.156170850284148</v>
       </c>
       <c r="G5">
-        <v>1.7375609346985701</v>
+        <v>1.73756093469857</v>
       </c>
       <c r="H5">
-        <v>-0.12958331175379689</v>
+        <v>-0.1295833117537969</v>
       </c>
       <c r="I5">
-        <v>3.6050411966872251</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+        <v>3.605041196687225</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -657,22 +590,22 @@
         <v>16</v>
       </c>
       <c r="E6">
-        <v>-2.6927441846377902</v>
+        <v>-2.69274418463779</v>
       </c>
       <c r="F6">
-        <v>-2.5906362887397361</v>
+        <v>-2.590636288739736</v>
       </c>
       <c r="G6">
         <v>-2.488528392841681</v>
       </c>
       <c r="H6">
-        <v>-2.7948520805358452</v>
+        <v>-2.794852080535845</v>
       </c>
       <c r="I6">
         <v>-2.386420496943626</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -689,19 +622,19 @@
         <v>1.215762212642878</v>
       </c>
       <c r="F7">
-        <v>1.3317420748383639</v>
+        <v>1.331742074838364</v>
       </c>
       <c r="G7">
-        <v>2.1040648029510511</v>
+        <v>2.104064802951051</v>
       </c>
       <c r="H7">
-        <v>0.32729161019060687</v>
+        <v>0.3272916101906069</v>
       </c>
       <c r="I7">
-        <v>3.1821347143092682</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+        <v>3.182134714309268</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -715,22 +648,22 @@
         <v>17</v>
       </c>
       <c r="E8">
-        <v>0.66487458854365322</v>
+        <v>0.6648745885436532</v>
       </c>
       <c r="F8">
-        <v>2.7471919816198311</v>
+        <v>2.747191981619831</v>
       </c>
       <c r="G8">
-        <v>3.1358779720039349</v>
+        <v>3.135877972003935</v>
       </c>
       <c r="H8">
         <v>-1.150421959812318</v>
       </c>
       <c r="I8">
-        <v>4.0333811776960866</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+        <v>4.033381177696087</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -744,22 +677,22 @@
         <v>17</v>
       </c>
       <c r="E9">
-        <v>-0.75198597635002429</v>
+        <v>-0.7519859763500243</v>
       </c>
       <c r="F9">
-        <v>-0.51527741295293528</v>
+        <v>-0.5152774129529353</v>
       </c>
       <c r="G9">
-        <v>0.16460658527874081</v>
+        <v>0.1646065852787408</v>
       </c>
       <c r="H9">
-        <v>-1.6570803967955541</v>
+        <v>-1.657080396795554</v>
       </c>
       <c r="I9">
         <v>0.5738884964150065</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -773,22 +706,22 @@
         <v>17</v>
       </c>
       <c r="E10">
-        <v>3.3629723089978989</v>
+        <v>3.362972308997899</v>
       </c>
       <c r="F10">
-        <v>3.9796255378050249</v>
+        <v>3.979625537805025</v>
       </c>
       <c r="G10">
         <v>5.327284281815631</v>
       </c>
       <c r="H10">
-        <v>2.8143341680431342</v>
+        <v>2.814334168043134</v>
       </c>
       <c r="I10">
-        <v>5.5127582969030691</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+        <v>5.512758296903069</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -805,19 +738,19 @@
         <v>-1.411640566900539</v>
       </c>
       <c r="F11">
-        <v>-0.81930427165020214</v>
+        <v>-0.8193042716502021</v>
       </c>
       <c r="G11">
-        <v>-0.16214289265810641</v>
+        <v>-0.1621428926581064</v>
       </c>
       <c r="H11">
         <v>-2.80875923981228</v>
       </c>
       <c r="I11">
-        <v>0.79311484834320856</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+        <v>0.7931148483432086</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -837,16 +770,16 @@
         <v>1.564668090199042</v>
       </c>
       <c r="G12">
-        <v>1.8360932410426389</v>
+        <v>1.836093241042639</v>
       </c>
       <c r="H12">
-        <v>1.0218177885118489</v>
+        <v>1.021817788511849</v>
       </c>
       <c r="I12">
-        <v>2.1075183918862348</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+        <v>2.107518391886235</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -860,22 +793,22 @@
         <v>17</v>
       </c>
       <c r="E13">
-        <v>-0.77415633365376779</v>
+        <v>-0.7741563336537678</v>
       </c>
       <c r="F13">
-        <v>2.247532107728592E-2</v>
+        <v>0.02247532107728592</v>
       </c>
       <c r="G13">
-        <v>0.69815215544928111</v>
+        <v>0.6981521554492811</v>
       </c>
       <c r="H13">
         <v>-1.575491063438309</v>
       </c>
       <c r="I13">
-        <v>1.4909774205975099</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+        <v>1.49097742059751</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -895,16 +828,16 @@
         <v>1.537346928585233</v>
       </c>
       <c r="G14">
-        <v>3.0325388474480639</v>
+        <v>3.032538847448064</v>
       </c>
       <c r="H14">
-        <v>-0.94609109760868126</v>
+        <v>-0.9460910976086813</v>
       </c>
       <c r="I14">
-        <v>4.9489588302181886</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+        <v>4.948958830218189</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -921,19 +854,19 @@
         <v>-0.473700121802</v>
       </c>
       <c r="F15">
-        <v>4.5808021216523637E-2</v>
+        <v>0.04580802121652364</v>
       </c>
       <c r="G15">
-        <v>0.43742738266649273</v>
+        <v>0.4374273826664927</v>
       </c>
       <c r="H15">
-        <v>-1.2868291775889309</v>
+        <v>-1.286829177588931</v>
       </c>
       <c r="I15">
-        <v>0.99219401015198483</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+        <v>0.9921940101519848</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -947,22 +880,22 @@
         <v>18</v>
       </c>
       <c r="E16">
-        <v>-1.9930245974042891</v>
+        <v>-1.993024597404289</v>
       </c>
       <c r="F16">
-        <v>0.19770219568517181</v>
+        <v>0.1977021956851718</v>
       </c>
       <c r="G16">
         <v>0.1997484888188423</v>
       </c>
       <c r="H16">
-        <v>-2.0194661857994149</v>
+        <v>-2.019466185799415</v>
       </c>
       <c r="I16">
-        <v>0.29245364895577908</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.2924536489557791</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -979,19 +912,19 @@
         <v>-1.420594714601692</v>
       </c>
       <c r="F17">
-        <v>-0.76603806727439405</v>
+        <v>-0.7660380672743941</v>
       </c>
       <c r="G17">
-        <v>-3.1449088685370913E-2</v>
+        <v>-0.03144908868537091</v>
       </c>
       <c r="H17">
-        <v>-2.8626796823236629</v>
+        <v>-2.862679682323663</v>
       </c>
       <c r="I17">
         <v>1.056177044728897</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1005,10 +938,10 @@
         <v>18</v>
       </c>
       <c r="E18">
-        <v>-2.7336400944530981</v>
+        <v>-2.733640094453098</v>
       </c>
       <c r="F18">
-        <v>-2.2443948437976902</v>
+        <v>-2.24439484379769</v>
       </c>
       <c r="G18">
         <v>-1.755149593142282</v>
@@ -1017,10 +950,10 @@
         <v>-3.222885345108506</v>
       </c>
       <c r="I18">
-        <v>-1.2659043424868739</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+        <v>-1.265904342486874</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1034,22 +967,22 @@
         <v>18</v>
       </c>
       <c r="E19">
-        <v>1.4354914455289911</v>
+        <v>1.435491445528991</v>
       </c>
       <c r="F19">
-        <v>2.1033221344001918</v>
+        <v>2.103322134400192</v>
       </c>
       <c r="G19">
-        <v>2.5085196113859212</v>
+        <v>2.508519611385921</v>
       </c>
       <c r="H19">
-        <v>0.52143810625597142</v>
+        <v>0.5214381062559714</v>
       </c>
       <c r="I19">
-        <v>2.8492140580319458</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+        <v>2.849214058031946</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1072,13 +1005,13 @@
         <v>2.885416216135575</v>
       </c>
       <c r="H20">
-        <v>-3.0653387896495121</v>
+        <v>-3.065338789649512</v>
       </c>
       <c r="I20">
-        <v>4.3420386712049597</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+        <v>4.34203867120496</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1092,22 +1025,22 @@
         <v>16</v>
       </c>
       <c r="E21">
-        <v>-2.2332244552982869</v>
+        <v>-2.233224455298287</v>
       </c>
       <c r="F21">
-        <v>-2.0763699166792922</v>
+        <v>-2.076369916679292</v>
       </c>
       <c r="G21">
         <v>-1.790606758917672</v>
       </c>
       <c r="H21">
-        <v>-2.6815626149214911</v>
+        <v>-2.681562614921491</v>
       </c>
       <c r="I21">
         <v>-1.302711936529579</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1124,7 +1057,7 @@
         <v>-1.320093727574803</v>
       </c>
       <c r="F22">
-        <v>0.23663223430289659</v>
+        <v>0.2366322343028966</v>
       </c>
       <c r="G22">
         <v>1.524556659036201</v>
@@ -1136,7 +1069,7 @@
         <v>3.435973417780378</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1150,22 +1083,22 @@
         <v>16</v>
       </c>
       <c r="E23">
-        <v>1.696497298305916E-2</v>
+        <v>0.01696497298305916</v>
       </c>
       <c r="F23">
-        <v>0.72391914728020734</v>
+        <v>0.7239191472802073</v>
       </c>
       <c r="G23">
-        <v>1.3469825007683289</v>
+        <v>1.346982500768329</v>
       </c>
       <c r="H23">
-        <v>-0.77426228236784289</v>
+        <v>-0.7742622823678429</v>
       </c>
       <c r="I23">
-        <v>2.8756905631072391</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+        <v>2.875690563107239</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1179,7 +1112,7 @@
         <v>16</v>
       </c>
       <c r="E24">
-        <v>-1.9889216813293511</v>
+        <v>-1.988921681329351</v>
       </c>
       <c r="F24">
         <v>-1.954040666535904</v>
@@ -1194,7 +1127,7 @@
         <v>-1.884278636949009</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1208,22 +1141,22 @@
         <v>16</v>
       </c>
       <c r="E25">
-        <v>0.91291490453417312</v>
+        <v>0.9129149045341731</v>
       </c>
       <c r="F25">
-        <v>1.2587271937870941</v>
+        <v>1.258727193787094</v>
       </c>
       <c r="G25">
-        <v>2.2186016094157268</v>
+        <v>2.218601609415727</v>
       </c>
       <c r="H25">
-        <v>-0.42893056813497799</v>
+        <v>-0.428930568134978</v>
       </c>
       <c r="I25">
         <v>3.390233270476243</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1243,16 +1176,16 @@
         <v>-0.3014084652093737</v>
       </c>
       <c r="G26">
-        <v>0.91688777030109492</v>
+        <v>0.9168877703010949</v>
       </c>
       <c r="H26">
-        <v>-3.8748722123222712</v>
+        <v>-3.874872212322271</v>
       </c>
       <c r="I26">
         <v>2.493721024115747</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1266,22 +1199,22 @@
         <v>17</v>
       </c>
       <c r="E27">
-        <v>-0.43169479947127459</v>
+        <v>-0.4316947994712746</v>
       </c>
       <c r="F27">
-        <v>7.0856264947809278E-2</v>
+        <v>0.07085626494780928</v>
       </c>
       <c r="G27">
-        <v>0.76623478146159885</v>
+        <v>0.7662347814615988</v>
       </c>
       <c r="H27">
         <v>-1.725321474324903</v>
       </c>
       <c r="I27">
-        <v>1.1998257420482039</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1.199825742048204</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1295,22 +1228,22 @@
         <v>17</v>
       </c>
       <c r="E28">
-        <v>2.9289957424536199</v>
+        <v>2.92899574245362</v>
       </c>
       <c r="F28">
         <v>3.448785025924864</v>
       </c>
       <c r="G28">
-        <v>3.7888194477875761</v>
+        <v>3.788819447787576</v>
       </c>
       <c r="H28">
-        <v>2.2785161775978029</v>
+        <v>2.278516177597803</v>
       </c>
       <c r="I28">
-        <v>4.2586379772284957</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+        <v>4.258637977228496</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1327,19 +1260,19 @@
         <v>-1.015777026423166</v>
       </c>
       <c r="F29">
-        <v>-3.1049458097841359E-2</v>
+        <v>-0.03104945809784136</v>
       </c>
       <c r="G29">
-        <v>0.60035446801076997</v>
+        <v>0.60035446801077</v>
       </c>
       <c r="H29">
-        <v>-2.2961648931440068</v>
+        <v>-2.296164893144007</v>
       </c>
       <c r="I29">
-        <v>1.9675964549464291</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1.967596454946429</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1353,7 +1286,7 @@
         <v>17</v>
       </c>
       <c r="E30">
-        <v>2.2026094267881908</v>
+        <v>2.202609426788191</v>
       </c>
       <c r="F30">
         <v>2.724173817711955</v>
@@ -1362,13 +1295,13 @@
         <v>3.24573820863572</v>
       </c>
       <c r="H30">
-        <v>1.6810450358644271</v>
+        <v>1.681045035864427</v>
       </c>
       <c r="I30">
-        <v>3.7673025995594842</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.767302599559484</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1382,22 +1315,22 @@
         <v>17</v>
       </c>
       <c r="E31">
-        <v>-2.3790514363002471</v>
+        <v>-2.379051436300247</v>
       </c>
       <c r="F31">
         <v>-1.766997322511201</v>
       </c>
       <c r="G31">
-        <v>-0.70187478655455759</v>
+        <v>-0.7018747865545576</v>
       </c>
       <c r="H31">
         <v>-2.579618891088451</v>
       </c>
       <c r="I31">
-        <v>0.36127753459762729</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.3612775345976273</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1411,22 +1344,22 @@
         <v>18</v>
       </c>
       <c r="E32">
-        <v>1.7208548588080541</v>
+        <v>1.720854858808054</v>
       </c>
       <c r="F32">
-        <v>2.4483579671819951</v>
+        <v>2.448357967181995</v>
       </c>
       <c r="G32">
-        <v>2.6349270622160872</v>
+        <v>2.634927062216087</v>
       </c>
       <c r="H32">
-        <v>0.60590727647979503</v>
+        <v>0.605907276479795</v>
       </c>
       <c r="I32">
-        <v>3.3283992458839129</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.328399245883913</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1440,22 +1373,22 @@
         <v>18</v>
       </c>
       <c r="E33">
-        <v>-0.12667499855005099</v>
+        <v>-0.126674998550051</v>
       </c>
       <c r="F33">
-        <v>9.8921050491331874E-2</v>
+        <v>0.09892105049133187</v>
       </c>
       <c r="G33">
-        <v>0.39178647890804841</v>
+        <v>0.3917864789080484</v>
       </c>
       <c r="H33">
-        <v>-0.40165419210272191</v>
+        <v>-0.4016541921027219</v>
       </c>
       <c r="I33">
-        <v>0.95256991798149293</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.9525699179814929</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1469,22 +1402,22 @@
         <v>18</v>
       </c>
       <c r="E34">
-        <v>1.1122338530490019</v>
+        <v>1.112233853049002</v>
       </c>
       <c r="F34">
-        <v>2.5904033878057939</v>
+        <v>2.590403387805794</v>
       </c>
       <c r="G34">
         <v>2.598946062050886</v>
       </c>
       <c r="H34">
-        <v>0.89550815224420255</v>
+        <v>0.8955081522442025</v>
       </c>
       <c r="I34">
-        <v>3.2521804684911491</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.252180468491149</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1498,22 +1431,22 @@
         <v>18</v>
       </c>
       <c r="E35">
-        <v>-1.7962100149831881</v>
+        <v>-1.796210014983188</v>
       </c>
       <c r="F35">
         <v>-1.168970101429865</v>
       </c>
       <c r="G35">
-        <v>-0.75836333648177567</v>
+        <v>-0.7583633364817757</v>
       </c>
       <c r="H35">
-        <v>-2.7073284933720609</v>
+        <v>-2.707328493372061</v>
       </c>
       <c r="I35">
-        <v>0.17020225465362099</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.170202254653621</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1527,22 +1460,22 @@
         <v>18</v>
       </c>
       <c r="E36">
-        <v>-0.93992441484693057</v>
+        <v>-0.9399244148469306</v>
       </c>
       <c r="F36">
-        <v>-0.73049018763333229</v>
+        <v>-0.7304901876333323</v>
       </c>
       <c r="G36">
-        <v>-0.52105596041973401</v>
+        <v>-0.521055960419734</v>
       </c>
       <c r="H36">
-        <v>-1.1493586420605291</v>
+        <v>-1.149358642060529</v>
       </c>
       <c r="I36">
-        <v>-0.31162173320613568</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+        <v>-0.3116217332061357</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1562,13 +1495,13 @@
         <v>1.327693284286477</v>
       </c>
       <c r="G37">
-        <v>1.5897106487187631</v>
+        <v>1.589710648718763</v>
       </c>
       <c r="H37">
-        <v>0.85971998986022413</v>
+        <v>0.8597199898602241</v>
       </c>
       <c r="I37">
-        <v>1.7295943545063071</v>
+        <v>1.729594354506307</v>
       </c>
     </row>
   </sheetData>

</xml_diff>